<commit_message>
add abgeordnetenwatch.de party manifesto links to link_manifestos
</commit_message>
<xml_diff>
--- a/inst/extdata/coldesc.xlsx
+++ b/inst/extdata/coldesc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/bundeslaendeR/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\addagwatch\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73313B89-3C7B-E241-86E1-ADEC2635E692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD25B6D8-685E-41C1-9776-7A0A4EAADA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="880" windowWidth="18000" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="2655" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>colname</t>
   </si>
@@ -476,6 +476,18 @@
   </si>
   <si>
     <t>election_remarks_wahlleiter</t>
+  </si>
+  <si>
+    <t>agwatch_pdf_url</t>
+  </si>
+  <si>
+    <t>agwatch_election_manifesto</t>
+  </si>
+  <si>
+    <t>Manifesto URL on abgeordnetenwatch.de</t>
+  </si>
+  <si>
+    <t>Is an electoral manifesto not just a general manifesto (AGWatch only)</t>
   </si>
 </sst>
 </file>
@@ -862,19 +874,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="67.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +894,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -890,7 +902,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -898,7 +910,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -906,7 +918,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -914,7 +926,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -922,7 +934,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -930,7 +942,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -938,7 +950,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -946,7 +958,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -954,7 +966,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -962,7 +974,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -970,7 +982,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -978,7 +990,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -986,7 +998,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1122,7 +1134,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1130,7 +1142,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1178,7 +1190,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1250,7 +1262,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1282,7 +1294,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1314,7 +1326,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1354,7 +1366,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1386,7 +1398,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1394,7 +1406,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1402,7 +1414,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1410,7 +1422,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1418,7 +1430,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1442,7 +1454,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1466,7 +1478,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1474,7 +1486,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1482,7 +1494,24 @@
         <v>150</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add pwib position data
</commit_message>
<xml_diff>
--- a/inst/extdata/coldesc.xlsx
+++ b/inst/extdata/coldesc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\addagwatch\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\blcbadd\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD25B6D8-685E-41C1-9776-7A0A4EAADA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E358A714-F835-4D57-AAC3-421581E3E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="2655" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>colname</t>
   </si>
@@ -488,6 +488,12 @@
   </si>
   <si>
     <t>Is an electoral manifesto not just a general manifesto (AGWatch only)</t>
+  </si>
+  <si>
+    <t>party_pwib</t>
+  </si>
+  <si>
+    <t>Partyname in PWIB policy position data</t>
   </si>
 </sst>
 </file>
@@ -874,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,6 +1516,14 @@
         <v>155</v>
       </c>
     </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add fortunato appeldorn legislative capacity data link
</commit_message>
<xml_diff>
--- a/inst/extdata/coldesc.xlsx
+++ b/inst/extdata/coldesc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\blcbadd\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\link_legcap\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E358A714-F835-4D57-AAC3-421581E3E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC37BE6-6F02-4069-A296-34DCC72DC17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="2655" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>colname</t>
   </si>
@@ -494,6 +494,18 @@
   </si>
   <si>
     <t>Partyname in PWIB policy position data</t>
+  </si>
+  <si>
+    <t>state_abb_appeldorn_fortunato</t>
+  </si>
+  <si>
+    <t>State abbreviation in Appeldorn and Fortunato's data</t>
+  </si>
+  <si>
+    <t>State name in Appeldorn and Fortunato's data</t>
+  </si>
+  <si>
+    <t>state_name_appeldorn_fortunato</t>
   </si>
 </sst>
 </file>
@@ -880,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,6 +1536,22 @@
         <v>157</v>
       </c>
     </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add legislative turnover data
</commit_message>
<xml_diff>
--- a/inst/extdata/coldesc.xlsx
+++ b/inst/extdata/coldesc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\link_legcap\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/bundeslaendeR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC37BE6-6F02-4069-A296-34DCC72DC17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1025D2-8089-AD47-B04F-EEDEE693645D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="2655" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25440" yWindow="5560" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>colname</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>state_name_appeldorn_fortunato</t>
+  </si>
+  <si>
+    <t>legislative_turnover_heinsohn</t>
+  </si>
+  <si>
+    <t>Legislative Turnover as measured by Heinsohn (2014)</t>
   </si>
 </sst>
 </file>
@@ -892,19 +898,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" customWidth="1"/>
-    <col min="2" max="2" width="67.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,7 +918,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -920,7 +926,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -928,7 +934,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -936,7 +942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -944,7 +950,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -952,7 +958,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -960,7 +966,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -968,7 +974,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -976,7 +982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -984,7 +990,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -992,7 +998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1080,7 +1086,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1120,7 +1126,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1150,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1198,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1216,7 +1222,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1238,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1344,7 +1350,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1360,7 +1366,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1392,7 +1398,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1408,7 +1414,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1424,7 +1430,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1432,7 +1438,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1448,7 +1454,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1480,7 +1486,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>153</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -1536,7 +1542,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -1544,12 +1550,20 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>161</v>
       </c>
       <c r="B81" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add link to integrated survey
</commit_message>
<xml_diff>
--- a/inst/extdata/coldesc.xlsx
+++ b/inst/extdata/coldesc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/bundeslaendeR/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\add\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1025D2-8089-AD47-B04F-EEDEE693645D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84423A52-3BA8-486B-AB17-3F933C7F9CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="5560" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2655" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t>colname</t>
   </si>
@@ -512,6 +512,30 @@
   </si>
   <si>
     <t>Legislative Turnover as measured by Heinsohn (2014)</t>
+  </si>
+  <si>
+    <t>bland</t>
+  </si>
+  <si>
+    <t>m7</t>
+  </si>
+  <si>
+    <t>m7b</t>
+  </si>
+  <si>
+    <t>za_nr1</t>
+  </si>
+  <si>
+    <t>State name in Integrated Survey Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey Party vote choice variable (from 1973 onwards) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey Party vote choice variable (until 1970) </t>
+  </si>
+  <si>
+    <t>ZA Dataset ID</t>
   </si>
 </sst>
 </file>
@@ -578,9 +602,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -618,9 +642,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,26 +677,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -705,26 +712,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -898,19 +888,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="67.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -926,7 +916,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -934,7 +924,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -942,7 +932,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -950,7 +940,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -958,7 +948,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -966,7 +956,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -974,7 +964,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -982,7 +972,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -990,7 +980,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -998,7 +988,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +996,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1004,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +1012,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1030,7 +1020,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1028,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1036,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1044,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1052,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1070,7 +1060,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1078,7 +1068,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1076,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1094,7 +1084,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1102,7 +1092,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1110,7 +1100,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1118,7 +1108,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1126,7 +1116,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1134,7 +1124,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1142,7 +1132,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1150,7 +1140,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1158,7 +1148,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1166,7 +1156,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1164,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1182,7 +1172,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1190,7 +1180,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1198,7 +1188,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1196,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1214,7 +1204,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1222,7 +1212,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1230,7 +1220,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1228,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1246,7 +1236,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1254,7 +1244,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1262,7 +1252,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1270,7 +1260,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1278,7 +1268,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1286,7 +1276,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1294,7 +1284,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1302,7 +1292,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1310,7 +1300,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1318,7 +1308,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1326,7 +1316,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1334,7 +1324,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1342,7 +1332,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1350,7 +1340,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1358,7 +1348,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1356,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1374,7 +1364,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1382,7 +1372,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1390,7 +1380,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1398,7 +1388,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1406,7 +1396,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1414,7 +1404,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1422,7 +1412,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1430,7 +1420,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1438,7 +1428,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1446,7 +1436,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1454,7 +1444,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1462,7 +1452,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1470,7 +1460,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1478,7 +1468,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1486,7 +1476,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1494,7 +1484,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1502,7 +1492,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1510,7 +1500,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1518,7 +1508,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -1526,7 +1516,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>153</v>
       </c>
@@ -1534,7 +1524,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -1542,7 +1532,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -1550,7 +1540,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -1558,12 +1548,44 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
       <c r="B82" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>